<commit_message>
Add desc stat and ICC to Chapter 4 Results
</commit_message>
<xml_diff>
--- a/Model building/Descriptive.xlsx
+++ b/Model building/Descriptive.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\MSc\Thesis\Model building\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E567A6CC-26D5-4360-BB6E-3786E3C56E53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE41ECB-DDED-4066-8E52-2315BFD5A830}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12840" windowWidth="18240" windowHeight="28440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Variable</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>level</t>
+  </si>
+  <si>
+    <t>FLIT</t>
   </si>
 </sst>
 </file>
@@ -507,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -597,7 +600,7 @@
         <v>96435</v>
       </c>
       <c r="D3" s="7">
-        <f>(107162-C3)/107162*100</f>
+        <f t="shared" ref="D3:D9" si="0">(107162-C3)/107162*100</f>
         <v>10.010078199361715</v>
       </c>
       <c r="E3" s="7"/>
@@ -639,7 +642,7 @@
         <v>95133</v>
       </c>
       <c r="D4" s="7">
-        <f>(107162-C4)/107162*100</f>
+        <f t="shared" si="0"/>
         <v>11.225061122412795</v>
       </c>
       <c r="E4" s="7"/>
@@ -650,7 +653,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" ref="H4:H14" si="0">SQRT(I4)</f>
+        <f t="shared" ref="H4:H17" si="1">SQRT(I4)</f>
         <v>1.0440306508910551</v>
       </c>
       <c r="I4" s="2">
@@ -678,7 +681,7 @@
         <v>83499</v>
       </c>
       <c r="D5" s="7">
-        <f>(107162-C5)/107162*100</f>
+        <f t="shared" si="0"/>
         <v>22.081521434836976</v>
       </c>
       <c r="E5" s="7"/>
@@ -689,7 +692,7 @@
         <v>-5.8999999999999997E-2</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0535653752852738</v>
       </c>
       <c r="I5" s="2">
@@ -710,131 +713,105 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>99969</v>
-      </c>
-      <c r="D6" s="7">
-        <f>(107162-C6)/107162*100</f>
-        <v>6.7122674082230649</v>
-      </c>
+      <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="2">
-        <v>7</v>
-      </c>
-      <c r="G6" s="2">
-        <v>7.0490000000000004</v>
-      </c>
-      <c r="H6" s="2">
-        <f t="shared" si="0"/>
-        <v>5.4545393939360265</v>
-      </c>
-      <c r="I6" s="2">
-        <v>29.751999999999999</v>
-      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="2">
-        <v>0.223</v>
-      </c>
-      <c r="L6" s="2">
-        <v>-1.0389999999999999</v>
-      </c>
-      <c r="M6" s="2">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2">
-        <v>18</v>
-      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>90130</v>
+        <v>104784</v>
       </c>
       <c r="D7" s="7">
         <f>(107162-C7)/107162*100</f>
-        <v>15.893693660066068</v>
+        <v>2.2190701927922212</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="2">
-        <v>-2.7E-2</v>
+        <v>-0.158</v>
       </c>
       <c r="G7" s="2">
-        <v>-7.1999999999999995E-2</v>
+        <v>-0.24099999999999999</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0168579055108928</v>
+        <f>SQRT(I7)</f>
+        <v>1.0876580344942983</v>
       </c>
       <c r="I7" s="2">
-        <v>1.034</v>
+        <v>1.1830000000000001</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2">
-        <v>-8.4000000000000005E-2</v>
+        <v>-0.53300000000000003</v>
       </c>
       <c r="L7" s="2">
-        <v>0.35499999999999998</v>
+        <v>0.184</v>
       </c>
       <c r="M7" s="2">
-        <v>-2.21</v>
+        <v>-7.7110000000000003</v>
       </c>
       <c r="N7" s="2">
-        <v>2.3220000000000001</v>
+        <v>4.234</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>104784</v>
+        <v>103317</v>
       </c>
       <c r="D8" s="7">
-        <f>(107162-C8)/107162*100</f>
-        <v>2.2190701927922212</v>
+        <f t="shared" ref="D8:D9" si="2">(107162-C8)/107162*100</f>
+        <v>3.5880256060917119</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="2">
-        <v>-0.158</v>
+        <v>0</v>
       </c>
       <c r="G8" s="2">
-        <v>-0.24099999999999999</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0876580344942983</v>
+        <f>SQRT(I8)</f>
+        <v>0.16733200530681511</v>
       </c>
       <c r="I8" s="2">
-        <v>1.1830000000000001</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2">
-        <v>-0.53300000000000003</v>
+        <v>5.6079999999999997</v>
       </c>
       <c r="L8" s="2">
-        <v>0.184</v>
+        <v>29.446000000000002</v>
       </c>
       <c r="M8" s="2">
-        <v>-7.7110000000000003</v>
+        <v>0</v>
       </c>
       <c r="N8" s="2">
-        <v>4.234</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>103317</v>
       </c>
       <c r="D9" s="7">
-        <f t="shared" ref="D9:D10" si="1">(107162-C9)/107162*100</f>
+        <f t="shared" si="2"/>
         <v>3.5880256060917119</v>
       </c>
       <c r="E9" s="7"/>
@@ -842,21 +819,21 @@
         <v>0</v>
       </c>
       <c r="G9" s="2">
-        <v>2.9000000000000001E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" si="0"/>
-        <v>0.16733200530681511</v>
+        <f>SQRT(I9)</f>
+        <v>0.20248456731316589</v>
       </c>
       <c r="I9" s="2">
-        <v>2.8000000000000001E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2">
-        <v>5.6079999999999997</v>
+        <v>4.5419999999999998</v>
       </c>
       <c r="L9" s="2">
-        <v>29.446000000000002</v>
+        <v>18.626999999999999</v>
       </c>
       <c r="M9" s="2">
         <v>0</v>
@@ -867,35 +844,35 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C10">
-        <v>103317</v>
+        <v>107160</v>
       </c>
       <c r="D10" s="7">
-        <f t="shared" si="1"/>
-        <v>3.5880256060917119</v>
+        <f>(107162-C10)/107162*100</f>
+        <v>1.8663332151322297E-3</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="2">
-        <v>4.2000000000000003E-2</v>
+        <v>0.502</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" si="0"/>
-        <v>0.20248456731316589</v>
+        <f>SQRT(I10)</f>
+        <v>0.5</v>
       </c>
       <c r="I10" s="2">
-        <v>4.1000000000000002E-2</v>
+        <v>0.25</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2">
-        <v>4.5419999999999998</v>
+        <v>-7.0000000000000001E-3</v>
       </c>
       <c r="L10" s="2">
-        <v>18.626999999999999</v>
+        <v>-2</v>
       </c>
       <c r="M10" s="2">
         <v>0</v>
@@ -905,153 +882,230 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>99969</v>
+      </c>
+      <c r="D12" s="7">
+        <f>(107162-C12)/107162*100</f>
+        <v>6.7122674082230649</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="2">
         <v>7</v>
       </c>
-      <c r="C11">
-        <v>107160</v>
-      </c>
-      <c r="D11" s="7">
-        <f>(107162-C11)/107162*100</f>
-        <v>1.8663332151322297E-3</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="2">
-        <v>1</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0.502</v>
-      </c>
-      <c r="H11" s="2">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2">
-        <v>-7.0000000000000001E-3</v>
-      </c>
-      <c r="L11" s="2">
-        <v>-2</v>
-      </c>
-      <c r="M11" s="2">
+      <c r="G12" s="2">
+        <v>7.0490000000000004</v>
+      </c>
+      <c r="H12" s="2">
+        <f>SQRT(I12)</f>
+        <v>5.4545393939360265</v>
+      </c>
+      <c r="I12" s="2">
+        <v>29.751999999999999</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2">
+        <v>0.223</v>
+      </c>
+      <c r="L12" s="2">
+        <v>-1.0389999999999999</v>
+      </c>
+      <c r="M12" s="2">
         <v>0</v>
       </c>
-      <c r="N11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
+      <c r="N12" s="2">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C13">
-        <v>6346</v>
+        <v>90130</v>
       </c>
       <c r="D13" s="7">
-        <f>(6631-C13)/6631*100</f>
-        <v>4.2979942693409736</v>
+        <f>(107162-C13)/107162*100</f>
+        <v>15.893693660066068</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="2">
-        <v>0.1</v>
+        <v>-2.7E-2</v>
       </c>
       <c r="G13" s="2">
-        <v>0.13100000000000001</v>
+        <v>-7.1999999999999995E-2</v>
       </c>
       <c r="H13" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0358571330062847</v>
+        <f>SQRT(I13)</f>
+        <v>1.0168579055108928</v>
       </c>
       <c r="I13" s="2">
-        <v>1.073</v>
+        <v>1.034</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2">
+        <v>-8.4000000000000005E-2</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="M13" s="2">
+        <v>-2.21</v>
+      </c>
+      <c r="N13" s="2">
+        <v>2.3220000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14">
+        <v>107162</v>
+      </c>
+      <c r="D14" s="7">
+        <f>(107162-C14)/107162*100</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="2">
+        <v>481.97</v>
+      </c>
+      <c r="G14" s="2">
+        <v>478.291</v>
+      </c>
+      <c r="H14" s="2">
+        <v>97.073999999999998</v>
+      </c>
+      <c r="I14" s="2">
+        <v>9423.32</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2">
+        <v>-8.8999999999999996E-2</v>
+      </c>
+      <c r="L14" s="2">
+        <v>-0.34</v>
+      </c>
+      <c r="M14" s="2">
+        <v>114.256</v>
+      </c>
+      <c r="N14" s="2">
+        <v>827.97699999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>6346</v>
+      </c>
+      <c r="D16" s="7">
+        <f>(6631-C16)/6631*100</f>
+        <v>4.2979942693409736</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0358571330062847</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1.073</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2">
         <v>0.34100000000000003</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L16" s="2">
         <v>-0.188</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M16" s="2">
         <v>-1.421</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N16" s="2">
         <v>2.9590000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C17" s="4">
         <v>5626</v>
       </c>
-      <c r="D14" s="8">
-        <f>(6631-C14)/6631*100</f>
+      <c r="D17" s="8">
+        <f>(6631-C17)/6631*100</f>
         <v>15.156085055044489</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="5">
+      <c r="E17" s="8"/>
+      <c r="F17" s="5">
         <v>11.885999999999999</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G17" s="5">
         <v>13.872999999999999</v>
       </c>
-      <c r="H14" s="5">
-        <f t="shared" si="0"/>
+      <c r="H17" s="5">
+        <f t="shared" si="1"/>
         <v>10.170988152583799</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I17" s="5">
         <v>103.449</v>
       </c>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5">
+      <c r="J17" s="5"/>
+      <c r="K17" s="5">
         <v>4.0209999999999999</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L17" s="5">
         <v>25.425000000000001</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M17" s="5">
         <v>1</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N17" s="5">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>